<commit_message>
model with ATLAS + Merck data
</commit_message>
<xml_diff>
--- a/ATLAS MODEL/ATLAS data.xlsx
+++ b/ATLAS MODEL/ATLAS data.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amber\Documents\Carbapenem\ATLAS MODEL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amber\Documents\Yale\CIDMA\AMR\Carbapenem-Resistance\ATLAS MODEL\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="6750"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="6750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resp_data" sheetId="9" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="HEENT" sheetId="5" r:id="rId7"/>
     <sheet name="INT" sheetId="7" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -165,7 +165,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -307,13 +307,13 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -595,19 +595,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:XFD36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="1" max="1" width="13.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
@@ -648,7 +648,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>12</v>
       </c>
@@ -689,7 +689,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>13</v>
       </c>
@@ -730,7 +730,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
         <v>14</v>
       </c>
@@ -771,7 +771,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>15</v>
       </c>
@@ -812,7 +812,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>16</v>
       </c>
@@ -853,7 +853,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
         <v>17</v>
       </c>
@@ -894,7 +894,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
         <v>26</v>
       </c>
@@ -935,7 +935,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
         <v>27</v>
       </c>
@@ -976,7 +976,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
         <v>18</v>
       </c>
@@ -1017,7 +1017,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
         <v>38</v>
       </c>
@@ -1042,7 +1042,7 @@
       <c r="L11" s="9"/>
       <c r="M11" s="12"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="11" t="s">
         <v>19</v>
       </c>
@@ -1083,7 +1083,7 @@
         <v>0.131918217</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="11" t="s">
         <v>20</v>
       </c>
@@ -1136,7 +1136,7 @@
         <v>0.1858974358974359</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="11" t="s">
         <v>21</v>
       </c>
@@ -1177,7 +1177,7 @@
         <v>0.16500000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="11" t="s">
         <v>22</v>
       </c>
@@ -1218,7 +1218,7 @@
         <v>0.10199999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" s="11" t="s">
         <v>23</v>
       </c>
@@ -1259,7 +1259,7 @@
         <v>6.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="11" t="s">
         <v>24</v>
       </c>
@@ -1300,7 +1300,7 @@
         <v>8.3000000000000004E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="11" t="s">
         <v>25</v>
       </c>
@@ -1341,7 +1341,7 @@
         <v>958682</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="11" t="s">
         <v>37</v>
       </c>
@@ -1356,20 +1356,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
-    <col min="2" max="2" width="8.140625" customWidth="1"/>
+    <col min="1" max="1" width="16.54296875" customWidth="1"/>
+    <col min="2" max="2" width="8.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
@@ -1410,7 +1410,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>12</v>
       </c>
@@ -1451,7 +1451,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>13</v>
       </c>
@@ -1492,7 +1492,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
         <v>14</v>
       </c>
@@ -1533,7 +1533,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>15</v>
       </c>
@@ -1574,7 +1574,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>16</v>
       </c>
@@ -1615,7 +1615,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
         <v>17</v>
       </c>
@@ -1656,7 +1656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
         <v>18</v>
       </c>
@@ -1697,7 +1697,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
         <v>38</v>
       </c>
@@ -1720,7 +1720,7 @@
       <c r="L9" s="9"/>
       <c r="M9" s="12"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
         <v>19</v>
       </c>
@@ -1761,7 +1761,7 @@
         <v>0.131918217</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="16" t="s">
         <v>36</v>
       </c>
@@ -1814,7 +1814,7 @@
         <v>0.14102564102564102</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="16" t="s">
         <v>34</v>
       </c>
@@ -1855,7 +1855,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="16" t="s">
         <v>35</v>
       </c>
@@ -1896,7 +1896,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="16" t="s">
         <v>33</v>
       </c>
@@ -1937,7 +1937,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="19" t="s">
         <v>25</v>
       </c>
@@ -1978,7 +1978,7 @@
         <v>958682</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" s="11" t="s">
         <v>37</v>
       </c>
@@ -1992,19 +1992,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
@@ -2045,7 +2045,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>12</v>
       </c>
@@ -2086,7 +2086,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>13</v>
       </c>
@@ -2127,7 +2127,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
         <v>14</v>
       </c>
@@ -2168,7 +2168,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>15</v>
       </c>
@@ -2209,7 +2209,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>16</v>
       </c>
@@ -2250,7 +2250,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
         <v>17</v>
       </c>
@@ -2291,7 +2291,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
         <v>18</v>
       </c>
@@ -2332,7 +2332,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
         <v>38</v>
       </c>
@@ -2355,7 +2355,7 @@
       <c r="L9" s="9"/>
       <c r="M9" s="12"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
         <v>19</v>
       </c>
@@ -2396,7 +2396,7 @@
         <v>0.131918217</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="16" t="s">
         <v>36</v>
       </c>
@@ -2449,7 +2449,7 @@
         <v>0.14102564102564102</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="16" t="s">
         <v>34</v>
       </c>
@@ -2490,7 +2490,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="16" t="s">
         <v>35</v>
       </c>
@@ -2531,7 +2531,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="16" t="s">
         <v>33</v>
       </c>
@@ -2572,7 +2572,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="19" t="s">
         <v>25</v>
       </c>
@@ -2613,7 +2613,7 @@
         <v>958682</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" s="11" t="s">
         <v>37</v>
       </c>
@@ -2627,84 +2627,84 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AB68"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A1" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="P1" s="23" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="P1" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="23"/>
-      <c r="S1" s="23"/>
-      <c r="T1" s="23"/>
-      <c r="U1" s="23"/>
-      <c r="V1" s="23"/>
-      <c r="W1" s="23"/>
-      <c r="X1" s="23"/>
-      <c r="Y1" s="23"/>
-      <c r="Z1" s="23"/>
-      <c r="AA1" s="23"/>
-      <c r="AB1" s="23"/>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+      <c r="W1" s="22"/>
+      <c r="X1" s="22"/>
+      <c r="Y1" s="22"/>
+      <c r="Z1" s="22"/>
+      <c r="AA1" s="22"/>
+      <c r="AB1" s="22"/>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A2" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
       <c r="G2" s="5"/>
-      <c r="H2" s="22" t="s">
+      <c r="H2" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
-      <c r="P2" s="22" t="s">
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+      <c r="P2" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="Q2" s="22"/>
-      <c r="R2" s="22"/>
-      <c r="S2" s="22"/>
-      <c r="T2" s="22"/>
-      <c r="U2" s="22"/>
+      <c r="Q2" s="21"/>
+      <c r="R2" s="21"/>
+      <c r="S2" s="21"/>
+      <c r="T2" s="21"/>
+      <c r="U2" s="21"/>
       <c r="V2" s="5"/>
-      <c r="W2" s="22" t="s">
+      <c r="W2" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="X2" s="22"/>
-      <c r="Y2" s="22"/>
-      <c r="Z2" s="22"/>
-      <c r="AA2" s="22"/>
-      <c r="AB2" s="22"/>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="X2" s="21"/>
+      <c r="Y2" s="21"/>
+      <c r="Z2" s="21"/>
+      <c r="AA2" s="21"/>
+      <c r="AB2" s="21"/>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -2778,7 +2778,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2004</v>
       </c>
@@ -2852,7 +2852,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>2005</v>
       </c>
@@ -2926,7 +2926,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>2006</v>
       </c>
@@ -3000,7 +3000,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>2007</v>
       </c>
@@ -3074,7 +3074,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>2008</v>
       </c>
@@ -3148,7 +3148,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>2009</v>
       </c>
@@ -3222,7 +3222,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>2010</v>
       </c>
@@ -3296,7 +3296,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>2011</v>
       </c>
@@ -3370,7 +3370,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>2012</v>
       </c>
@@ -3444,7 +3444,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>2013</v>
       </c>
@@ -3518,7 +3518,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>2014</v>
       </c>
@@ -3592,7 +3592,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>2015</v>
       </c>
@@ -3666,7 +3666,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A16" s="7">
         <v>2016</v>
       </c>
@@ -3742,39 +3742,39 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="P17" s="1"/>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A18" s="22" t="s">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A18" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="22"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
       <c r="G18" s="3"/>
-      <c r="H18" s="22" t="s">
+      <c r="H18" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
-      <c r="K18" s="22"/>
-      <c r="L18" s="22"/>
-      <c r="M18" s="22"/>
-      <c r="P18" s="22" t="s">
+      <c r="I18" s="21"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="21"/>
+      <c r="L18" s="21"/>
+      <c r="M18" s="21"/>
+      <c r="P18" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="Q18" s="22"/>
-      <c r="R18" s="22"/>
-      <c r="S18" s="22"/>
-      <c r="T18" s="22"/>
-      <c r="U18" s="22"/>
+      <c r="Q18" s="21"/>
+      <c r="R18" s="21"/>
+      <c r="S18" s="21"/>
+      <c r="T18" s="21"/>
+      <c r="U18" s="21"/>
       <c r="V18" s="3"/>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A19" s="6" t="s">
         <v>1</v>
       </c>
@@ -3830,7 +3830,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>2004</v>
       </c>
@@ -3886,7 +3886,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>2005</v>
       </c>
@@ -3942,7 +3942,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>2006</v>
       </c>
@@ -3998,7 +3998,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>2007</v>
       </c>
@@ -4054,7 +4054,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>2008</v>
       </c>
@@ -4110,7 +4110,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>2009</v>
       </c>
@@ -4166,7 +4166,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>2010</v>
       </c>
@@ -4222,7 +4222,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>2011</v>
       </c>
@@ -4278,7 +4278,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>2012</v>
       </c>
@@ -4334,7 +4334,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>2013</v>
       </c>
@@ -4390,7 +4390,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>2014</v>
       </c>
@@ -4446,7 +4446,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>2015</v>
       </c>
@@ -4502,7 +4502,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A32" s="7">
         <v>2016</v>
       </c>
@@ -4560,59 +4560,59 @@
       </c>
       <c r="V32" s="3"/>
     </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A37" s="21" t="s">
+    <row r="37" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A37" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="B37" s="21"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="21"/>
-      <c r="E37" s="21"/>
-      <c r="F37" s="21"/>
-      <c r="P37" s="23" t="s">
+      <c r="B37" s="23"/>
+      <c r="C37" s="23"/>
+      <c r="D37" s="23"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="23"/>
+      <c r="P37" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="Q37" s="23"/>
-      <c r="R37" s="23"/>
-      <c r="S37" s="23"/>
-      <c r="T37" s="23"/>
-      <c r="U37" s="23"/>
-      <c r="V37" s="23"/>
-      <c r="W37" s="23"/>
-      <c r="X37" s="23"/>
-      <c r="Y37" s="23"/>
-      <c r="Z37" s="23"/>
-      <c r="AA37" s="23"/>
-      <c r="AB37" s="23"/>
-    </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A38" s="22" t="s">
+      <c r="Q37" s="22"/>
+      <c r="R37" s="22"/>
+      <c r="S37" s="22"/>
+      <c r="T37" s="22"/>
+      <c r="U37" s="22"/>
+      <c r="V37" s="22"/>
+      <c r="W37" s="22"/>
+      <c r="X37" s="22"/>
+      <c r="Y37" s="22"/>
+      <c r="Z37" s="22"/>
+      <c r="AA37" s="22"/>
+      <c r="AB37" s="22"/>
+    </row>
+    <row r="38" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A38" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B38" s="22"/>
-      <c r="C38" s="22"/>
-      <c r="D38" s="22"/>
-      <c r="E38" s="22"/>
-      <c r="F38" s="22"/>
-      <c r="P38" s="22" t="s">
+      <c r="B38" s="21"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="21"/>
+      <c r="P38" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="Q38" s="22"/>
-      <c r="R38" s="22"/>
-      <c r="S38" s="22"/>
-      <c r="T38" s="22"/>
-      <c r="U38" s="22"/>
+      <c r="Q38" s="21"/>
+      <c r="R38" s="21"/>
+      <c r="S38" s="21"/>
+      <c r="T38" s="21"/>
+      <c r="U38" s="21"/>
       <c r="V38" s="5"/>
-      <c r="W38" s="22" t="s">
+      <c r="W38" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="X38" s="22"/>
-      <c r="Y38" s="22"/>
-      <c r="Z38" s="22"/>
-      <c r="AA38" s="22"/>
-      <c r="AB38" s="22"/>
-    </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="X38" s="21"/>
+      <c r="Y38" s="21"/>
+      <c r="Z38" s="21"/>
+      <c r="AA38" s="21"/>
+      <c r="AB38" s="21"/>
+    </row>
+    <row r="39" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A39" s="6" t="s">
         <v>1</v>
       </c>
@@ -4668,7 +4668,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>2004</v>
       </c>
@@ -4724,7 +4724,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>2005</v>
       </c>
@@ -4780,7 +4780,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>2006</v>
       </c>
@@ -4836,7 +4836,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>2007</v>
       </c>
@@ -4892,7 +4892,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>2008</v>
       </c>
@@ -4948,7 +4948,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>2009</v>
       </c>
@@ -5004,7 +5004,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="46" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>2010</v>
       </c>
@@ -5060,7 +5060,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>2011</v>
       </c>
@@ -5116,7 +5116,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>2012</v>
       </c>
@@ -5172,7 +5172,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="49" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>2013</v>
       </c>
@@ -5228,7 +5228,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="50" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
         <v>2014</v>
       </c>
@@ -5284,7 +5284,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="51" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
         <v>2015</v>
       </c>
@@ -5340,7 +5340,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="52" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A52" s="7">
         <v>2016</v>
       </c>
@@ -5397,21 +5397,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:28" x14ac:dyDescent="0.35">
       <c r="P53" s="1"/>
     </row>
-    <row r="54" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="P54" s="22" t="s">
+    <row r="54" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="P54" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="Q54" s="22"/>
-      <c r="R54" s="22"/>
-      <c r="S54" s="22"/>
-      <c r="T54" s="22"/>
-      <c r="U54" s="22"/>
+      <c r="Q54" s="21"/>
+      <c r="R54" s="21"/>
+      <c r="S54" s="21"/>
+      <c r="T54" s="21"/>
+      <c r="U54" s="21"/>
       <c r="V54" s="3"/>
     </row>
-    <row r="55" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:28" x14ac:dyDescent="0.35">
       <c r="P55" s="6" t="s">
         <v>1</v>
       </c>
@@ -5431,7 +5431,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="56" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:28" x14ac:dyDescent="0.35">
       <c r="P56" s="1">
         <v>2004</v>
       </c>
@@ -5451,7 +5451,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:28" x14ac:dyDescent="0.35">
       <c r="P57" s="1">
         <v>2005</v>
       </c>
@@ -5471,7 +5471,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:28" x14ac:dyDescent="0.35">
       <c r="P58" s="1">
         <v>2006</v>
       </c>
@@ -5491,7 +5491,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:28" x14ac:dyDescent="0.35">
       <c r="P59" s="1">
         <v>2007</v>
       </c>
@@ -5511,7 +5511,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="60" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:28" x14ac:dyDescent="0.35">
       <c r="P60" s="1">
         <v>2008</v>
       </c>
@@ -5531,7 +5531,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:28" x14ac:dyDescent="0.35">
       <c r="P61" s="1">
         <v>2009</v>
       </c>
@@ -5551,7 +5551,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:28" x14ac:dyDescent="0.35">
       <c r="P62" s="1">
         <v>2010</v>
       </c>
@@ -5571,7 +5571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:28" x14ac:dyDescent="0.35">
       <c r="P63" s="1">
         <v>2011</v>
       </c>
@@ -5591,7 +5591,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:28" x14ac:dyDescent="0.35">
       <c r="P64" s="1">
         <v>2012</v>
       </c>
@@ -5611,7 +5611,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="16:22" x14ac:dyDescent="0.25">
+    <row r="65" spans="16:22" x14ac:dyDescent="0.35">
       <c r="P65" s="1">
         <v>2013</v>
       </c>
@@ -5631,7 +5631,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="16:22" x14ac:dyDescent="0.25">
+    <row r="66" spans="16:22" x14ac:dyDescent="0.35">
       <c r="P66" s="1">
         <v>2014</v>
       </c>
@@ -5651,7 +5651,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="16:22" x14ac:dyDescent="0.25">
+    <row r="67" spans="16:22" x14ac:dyDescent="0.35">
       <c r="P67" s="1">
         <v>2015</v>
       </c>
@@ -5671,7 +5671,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="16:22" x14ac:dyDescent="0.25">
+    <row r="68" spans="16:22" x14ac:dyDescent="0.35">
       <c r="P68" s="7">
         <v>2016</v>
       </c>
@@ -5715,7 +5715,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -5725,79 +5725,79 @@
       <selection activeCell="A35" sqref="A35:M66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="O1" s="23" t="s">
+    <row r="1" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="O1" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="23"/>
-      <c r="S1" s="23"/>
-      <c r="T1" s="23"/>
-      <c r="U1" s="23"/>
-      <c r="V1" s="23"/>
-      <c r="W1" s="23"/>
-      <c r="X1" s="23"/>
-      <c r="Y1" s="23"/>
-      <c r="Z1" s="23"/>
-      <c r="AA1" s="23"/>
-    </row>
-    <row r="2" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+      <c r="W1" s="22"/>
+      <c r="X1" s="22"/>
+      <c r="Y1" s="22"/>
+      <c r="Z1" s="22"/>
+      <c r="AA1" s="22"/>
+    </row>
+    <row r="2" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
       <c r="G2" s="5"/>
-      <c r="H2" s="22" t="s">
+      <c r="H2" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
-      <c r="O2" s="22" t="s">
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+      <c r="O2" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="P2" s="22"/>
-      <c r="Q2" s="22"/>
-      <c r="R2" s="22"/>
-      <c r="S2" s="22"/>
-      <c r="T2" s="22"/>
-      <c r="V2" s="22" t="s">
+      <c r="P2" s="21"/>
+      <c r="Q2" s="21"/>
+      <c r="R2" s="21"/>
+      <c r="S2" s="21"/>
+      <c r="T2" s="21"/>
+      <c r="V2" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="W2" s="22"/>
-      <c r="X2" s="22"/>
-      <c r="Y2" s="22"/>
-      <c r="Z2" s="22"/>
-      <c r="AA2" s="22"/>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="W2" s="21"/>
+      <c r="X2" s="21"/>
+      <c r="Y2" s="21"/>
+      <c r="Z2" s="21"/>
+      <c r="AA2" s="21"/>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -5871,7 +5871,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2004</v>
       </c>
@@ -5945,7 +5945,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>2005</v>
       </c>
@@ -6019,7 +6019,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>2006</v>
       </c>
@@ -6093,7 +6093,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>2007</v>
       </c>
@@ -6167,7 +6167,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>2008</v>
       </c>
@@ -6241,7 +6241,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>2009</v>
       </c>
@@ -6315,7 +6315,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>2010</v>
       </c>
@@ -6389,7 +6389,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>2011</v>
       </c>
@@ -6463,7 +6463,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>2012</v>
       </c>
@@ -6537,7 +6537,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>2013</v>
       </c>
@@ -6611,7 +6611,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>2014</v>
       </c>
@@ -6685,7 +6685,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>2015</v>
       </c>
@@ -6759,7 +6759,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A16" s="7">
         <v>2016</v>
       </c>
@@ -6834,45 +6834,45 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.35">
       <c r="O17" s="1"/>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A18" s="22" t="s">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A18" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="22"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
       <c r="G18" s="3"/>
-      <c r="H18" s="22" t="s">
+      <c r="H18" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
-      <c r="K18" s="22"/>
-      <c r="L18" s="22"/>
-      <c r="M18" s="22"/>
-      <c r="O18" s="22" t="s">
+      <c r="I18" s="21"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="21"/>
+      <c r="L18" s="21"/>
+      <c r="M18" s="21"/>
+      <c r="O18" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="P18" s="22"/>
-      <c r="Q18" s="22"/>
-      <c r="R18" s="22"/>
-      <c r="S18" s="22"/>
-      <c r="T18" s="22"/>
-      <c r="V18" s="22" t="s">
+      <c r="P18" s="21"/>
+      <c r="Q18" s="21"/>
+      <c r="R18" s="21"/>
+      <c r="S18" s="21"/>
+      <c r="T18" s="21"/>
+      <c r="V18" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="W18" s="22"/>
-      <c r="X18" s="22"/>
-      <c r="Y18" s="22"/>
-      <c r="Z18" s="22"/>
-      <c r="AA18" s="22"/>
-    </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="W18" s="21"/>
+      <c r="X18" s="21"/>
+      <c r="Y18" s="21"/>
+      <c r="Z18" s="21"/>
+      <c r="AA18" s="21"/>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A19" s="6" t="s">
         <v>1</v>
       </c>
@@ -6946,7 +6946,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>2004</v>
       </c>
@@ -7020,7 +7020,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>2005</v>
       </c>
@@ -7094,7 +7094,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>2006</v>
       </c>
@@ -7168,7 +7168,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>2007</v>
       </c>
@@ -7242,7 +7242,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>2008</v>
       </c>
@@ -7316,7 +7316,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>2009</v>
       </c>
@@ -7390,7 +7390,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>2010</v>
       </c>
@@ -7464,7 +7464,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>2011</v>
       </c>
@@ -7538,7 +7538,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>2012</v>
       </c>
@@ -7612,7 +7612,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>2013</v>
       </c>
@@ -7686,7 +7686,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>2014</v>
       </c>
@@ -7760,7 +7760,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>2015</v>
       </c>
@@ -7834,7 +7834,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A32" s="7">
         <v>2016</v>
       </c>
@@ -7909,46 +7909,46 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" s="23" t="s">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A35" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="B35" s="23"/>
-      <c r="C35" s="23"/>
-      <c r="D35" s="23"/>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
-      <c r="G35" s="23"/>
-      <c r="H35" s="23"/>
-      <c r="I35" s="23"/>
-      <c r="J35" s="23"/>
-      <c r="K35" s="23"/>
-      <c r="L35" s="23"/>
-      <c r="M35" s="23"/>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="22" t="s">
+      <c r="B35" s="22"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="22"/>
+      <c r="J35" s="22"/>
+      <c r="K35" s="22"/>
+      <c r="L35" s="22"/>
+      <c r="M35" s="22"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A36" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B36" s="22"/>
-      <c r="C36" s="22"/>
-      <c r="D36" s="22"/>
-      <c r="E36" s="22"/>
-      <c r="F36" s="22"/>
+      <c r="B36" s="21"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
       <c r="G36" s="5"/>
-      <c r="H36" s="22" t="s">
+      <c r="H36" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="22"/>
-      <c r="J36" s="22"/>
-      <c r="K36" s="22"/>
-      <c r="L36" s="22"/>
-      <c r="M36" s="22"/>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I36" s="21"/>
+      <c r="J36" s="21"/>
+      <c r="K36" s="21"/>
+      <c r="L36" s="21"/>
+      <c r="M36" s="21"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37" s="6" t="s">
         <v>1</v>
       </c>
@@ -7986,7 +7986,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>2004</v>
       </c>
@@ -8024,7 +8024,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>2005</v>
       </c>
@@ -8062,7 +8062,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>2006</v>
       </c>
@@ -8100,7 +8100,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>2007</v>
       </c>
@@ -8138,7 +8138,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>2008</v>
       </c>
@@ -8176,7 +8176,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>2009</v>
       </c>
@@ -8214,7 +8214,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>2010</v>
       </c>
@@ -8252,7 +8252,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>2011</v>
       </c>
@@ -8290,7 +8290,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>2012</v>
       </c>
@@ -8328,7 +8328,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>2013</v>
       </c>
@@ -8366,7 +8366,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>2014</v>
       </c>
@@ -8404,7 +8404,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>2015</v>
       </c>
@@ -8442,7 +8442,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A50" s="7">
         <v>2016</v>
       </c>
@@ -8481,26 +8481,26 @@
         <v>16</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A52" s="22" t="s">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A52" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B52" s="22"/>
-      <c r="C52" s="22"/>
-      <c r="D52" s="22"/>
-      <c r="E52" s="22"/>
-      <c r="F52" s="22"/>
+      <c r="B52" s="21"/>
+      <c r="C52" s="21"/>
+      <c r="D52" s="21"/>
+      <c r="E52" s="21"/>
+      <c r="F52" s="21"/>
       <c r="G52" s="3"/>
-      <c r="H52" s="22" t="s">
+      <c r="H52" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="I52" s="22"/>
-      <c r="J52" s="22"/>
-      <c r="K52" s="22"/>
-      <c r="L52" s="22"/>
-      <c r="M52" s="22"/>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I52" s="21"/>
+      <c r="J52" s="21"/>
+      <c r="K52" s="21"/>
+      <c r="L52" s="21"/>
+      <c r="M52" s="21"/>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A53" s="6" t="s">
         <v>1</v>
       </c>
@@ -8538,7 +8538,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
         <v>2004</v>
       </c>
@@ -8576,7 +8576,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
         <v>2005</v>
       </c>
@@ -8614,7 +8614,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
         <v>2006</v>
       </c>
@@ -8652,7 +8652,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
         <v>2007</v>
       </c>
@@ -8690,7 +8690,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
         <v>2008</v>
       </c>
@@ -8728,7 +8728,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
         <v>2009</v>
       </c>
@@ -8766,7 +8766,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
         <v>2010</v>
       </c>
@@ -8804,7 +8804,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
         <v>2011</v>
       </c>
@@ -8842,7 +8842,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
         <v>2012</v>
       </c>
@@ -8880,7 +8880,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
         <v>2013</v>
       </c>
@@ -8918,7 +8918,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
         <v>2014</v>
       </c>
@@ -8956,7 +8956,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <v>2015</v>
       </c>
@@ -8994,7 +8994,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A66" s="7">
         <v>2016</v>
       </c>
@@ -9033,10 +9033,10 @@
         <v>14</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A67"/>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A68"/>
     </row>
   </sheetData>
@@ -9066,7 +9066,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -9076,79 +9076,79 @@
       <selection activeCell="A35" sqref="A35:M66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
+    <row r="1" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A1" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
       <c r="N1" s="2"/>
-      <c r="O1" s="23" t="s">
+      <c r="O1" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="23"/>
-      <c r="S1" s="23"/>
-      <c r="T1" s="23"/>
-      <c r="U1" s="23"/>
-      <c r="V1" s="23"/>
-      <c r="W1" s="23"/>
-      <c r="X1" s="23"/>
-      <c r="Y1" s="23"/>
-      <c r="Z1" s="23"/>
-      <c r="AA1" s="23"/>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+      <c r="W1" s="22"/>
+      <c r="X1" s="22"/>
+      <c r="Y1" s="22"/>
+      <c r="Z1" s="22"/>
+      <c r="AA1" s="22"/>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A2" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
       <c r="G2" s="5"/>
-      <c r="H2" s="22" t="s">
+      <c r="H2" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
       <c r="N2" s="2"/>
-      <c r="O2" s="22" t="s">
+      <c r="O2" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="P2" s="22"/>
-      <c r="Q2" s="22"/>
-      <c r="R2" s="22"/>
-      <c r="S2" s="22"/>
-      <c r="T2" s="22"/>
+      <c r="P2" s="21"/>
+      <c r="Q2" s="21"/>
+      <c r="R2" s="21"/>
+      <c r="S2" s="21"/>
+      <c r="T2" s="21"/>
       <c r="U2" s="2"/>
-      <c r="V2" s="22" t="s">
+      <c r="V2" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="W2" s="22"/>
-      <c r="X2" s="22"/>
-      <c r="Y2" s="22"/>
-      <c r="Z2" s="22"/>
-      <c r="AA2" s="22"/>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="W2" s="21"/>
+      <c r="X2" s="21"/>
+      <c r="Y2" s="21"/>
+      <c r="Z2" s="21"/>
+      <c r="AA2" s="21"/>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -9222,7 +9222,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2004</v>
       </c>
@@ -9296,7 +9296,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>2005</v>
       </c>
@@ -9370,7 +9370,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>2006</v>
       </c>
@@ -9444,7 +9444,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>2007</v>
       </c>
@@ -9518,7 +9518,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>2008</v>
       </c>
@@ -9592,7 +9592,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>2009</v>
       </c>
@@ -9666,7 +9666,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>2010</v>
       </c>
@@ -9740,7 +9740,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>2011</v>
       </c>
@@ -9799,7 +9799,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>2012</v>
       </c>
@@ -9873,7 +9873,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>2013</v>
       </c>
@@ -9947,7 +9947,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>2014</v>
       </c>
@@ -10006,7 +10006,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>2015</v>
       </c>
@@ -10080,7 +10080,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A16" s="7">
         <v>2016</v>
       </c>
@@ -10135,30 +10135,30 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="O17" s="1"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="22" t="s">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A18" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="22"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
       <c r="G18" s="3"/>
-      <c r="O18" s="22" t="s">
+      <c r="O18" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="P18" s="22"/>
-      <c r="Q18" s="22"/>
-      <c r="R18" s="22"/>
-      <c r="S18" s="22"/>
-      <c r="T18" s="22"/>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="P18" s="21"/>
+      <c r="Q18" s="21"/>
+      <c r="R18" s="21"/>
+      <c r="S18" s="21"/>
+      <c r="T18" s="21"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A19" s="6" t="s">
         <v>1</v>
       </c>
@@ -10196,7 +10196,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>2004</v>
       </c>
@@ -10234,7 +10234,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>2005</v>
       </c>
@@ -10272,7 +10272,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>2006</v>
       </c>
@@ -10310,7 +10310,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>2007</v>
       </c>
@@ -10348,7 +10348,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>2008</v>
       </c>
@@ -10386,7 +10386,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>2009</v>
       </c>
@@ -10424,7 +10424,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>2010</v>
       </c>
@@ -10462,7 +10462,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>2011</v>
       </c>
@@ -10500,7 +10500,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>2012</v>
       </c>
@@ -10538,7 +10538,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>2013</v>
       </c>
@@ -10576,7 +10576,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>2014</v>
       </c>
@@ -10614,7 +10614,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>2015</v>
       </c>
@@ -10652,7 +10652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A32" s="7">
         <v>2016</v>
       </c>
@@ -10691,43 +10691,43 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" s="23" t="s">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A35" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="B35" s="23"/>
-      <c r="C35" s="23"/>
-      <c r="D35" s="23"/>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
-      <c r="G35" s="23"/>
-      <c r="H35" s="23"/>
-      <c r="I35" s="23"/>
-      <c r="J35" s="23"/>
-      <c r="K35" s="23"/>
-      <c r="L35" s="23"/>
-      <c r="M35" s="23"/>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="22" t="s">
+      <c r="B35" s="22"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="22"/>
+      <c r="J35" s="22"/>
+      <c r="K35" s="22"/>
+      <c r="L35" s="22"/>
+      <c r="M35" s="22"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A36" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B36" s="22"/>
-      <c r="C36" s="22"/>
-      <c r="D36" s="22"/>
-      <c r="E36" s="22"/>
-      <c r="F36" s="22"/>
+      <c r="B36" s="21"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
       <c r="G36" s="5"/>
-      <c r="H36" s="22" t="s">
+      <c r="H36" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="22"/>
-      <c r="J36" s="22"/>
-      <c r="K36" s="22"/>
-      <c r="L36" s="22"/>
-      <c r="M36" s="22"/>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I36" s="21"/>
+      <c r="J36" s="21"/>
+      <c r="K36" s="21"/>
+      <c r="L36" s="21"/>
+      <c r="M36" s="21"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37" s="6" t="s">
         <v>1</v>
       </c>
@@ -10765,7 +10765,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>2004</v>
       </c>
@@ -10803,7 +10803,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>2005</v>
       </c>
@@ -10841,7 +10841,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>2006</v>
       </c>
@@ -10879,7 +10879,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>2007</v>
       </c>
@@ -10917,7 +10917,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>2008</v>
       </c>
@@ -10955,7 +10955,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>2009</v>
       </c>
@@ -10993,7 +10993,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>2010</v>
       </c>
@@ -11031,7 +11031,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>2011</v>
       </c>
@@ -11069,7 +11069,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>2012</v>
       </c>
@@ -11107,7 +11107,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>2013</v>
       </c>
@@ -11145,7 +11145,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>2014</v>
       </c>
@@ -11183,7 +11183,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>2015</v>
       </c>
@@ -11221,7 +11221,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A50" s="7">
         <v>2016</v>
       </c>
@@ -11260,21 +11260,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A51" s="1"/>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A52" s="22" t="s">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A52" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B52" s="22"/>
-      <c r="C52" s="22"/>
-      <c r="D52" s="22"/>
-      <c r="E52" s="22"/>
-      <c r="F52" s="22"/>
+      <c r="B52" s="21"/>
+      <c r="C52" s="21"/>
+      <c r="D52" s="21"/>
+      <c r="E52" s="21"/>
+      <c r="F52" s="21"/>
       <c r="G52" s="3"/>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A53" s="6" t="s">
         <v>1</v>
       </c>
@@ -11294,7 +11294,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
         <v>2004</v>
       </c>
@@ -11314,7 +11314,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
         <v>2005</v>
       </c>
@@ -11334,7 +11334,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
         <v>2006</v>
       </c>
@@ -11354,7 +11354,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
         <v>2007</v>
       </c>
@@ -11374,7 +11374,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
         <v>2008</v>
       </c>
@@ -11394,7 +11394,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
         <v>2009</v>
       </c>
@@ -11414,7 +11414,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
         <v>2010</v>
       </c>
@@ -11434,7 +11434,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
         <v>2011</v>
       </c>
@@ -11454,7 +11454,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
         <v>2012</v>
       </c>
@@ -11474,7 +11474,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
         <v>2013</v>
       </c>
@@ -11494,7 +11494,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
         <v>2014</v>
       </c>
@@ -11514,7 +11514,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <v>2015</v>
       </c>
@@ -11534,7 +11534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A66" s="7">
         <v>2016</v>
       </c>
@@ -11579,7 +11579,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -11589,63 +11589,63 @@
       <selection activeCell="O1" sqref="O1:T16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="H1" s="21" t="s">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="H1" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
       <c r="N1" s="2"/>
-      <c r="O1" s="21" t="s">
+      <c r="O1" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21"/>
-      <c r="R1" s="21"/>
-      <c r="S1" s="21"/>
-      <c r="T1" s="21"/>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="23"/>
+      <c r="S1" s="23"/>
+      <c r="T1" s="23"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A2" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="H2" s="22" t="s">
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="H2" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
       <c r="N2" s="2"/>
-      <c r="O2" s="22" t="s">
+      <c r="O2" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="P2" s="22"/>
-      <c r="Q2" s="22"/>
-      <c r="R2" s="22"/>
-      <c r="S2" s="22"/>
-      <c r="T2" s="22"/>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="P2" s="21"/>
+      <c r="Q2" s="21"/>
+      <c r="R2" s="21"/>
+      <c r="S2" s="21"/>
+      <c r="T2" s="21"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -11701,7 +11701,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2004</v>
       </c>
@@ -11757,7 +11757,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>2005</v>
       </c>
@@ -11813,7 +11813,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>2006</v>
       </c>
@@ -11869,7 +11869,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>2007</v>
       </c>
@@ -11925,7 +11925,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>2008</v>
       </c>
@@ -11966,7 +11966,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>2009</v>
       </c>
@@ -12022,7 +12022,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>2010</v>
       </c>
@@ -12078,7 +12078,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>2011</v>
       </c>
@@ -12134,7 +12134,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>2012</v>
       </c>
@@ -12190,7 +12190,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>2013</v>
       </c>
@@ -12231,7 +12231,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>2014</v>
       </c>
@@ -12272,7 +12272,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>2015</v>
       </c>
@@ -12313,7 +12313,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A16" s="7">
         <v>2016</v>
       </c>
@@ -12360,7 +12360,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
     </row>
   </sheetData>
@@ -12381,89 +12381,89 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AA67"/>
   <sheetViews>
     <sheetView topLeftCell="C7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D67" sqref="D67"/>
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
+    <row r="1" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A1" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
       <c r="N1" s="2"/>
-      <c r="O1" s="23" t="s">
+      <c r="O1" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="23"/>
-      <c r="S1" s="23"/>
-      <c r="T1" s="23"/>
-      <c r="U1" s="23"/>
-      <c r="V1" s="23"/>
-      <c r="W1" s="23"/>
-      <c r="X1" s="23"/>
-      <c r="Y1" s="23"/>
-      <c r="Z1" s="23"/>
-      <c r="AA1" s="23"/>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+      <c r="W1" s="22"/>
+      <c r="X1" s="22"/>
+      <c r="Y1" s="22"/>
+      <c r="Z1" s="22"/>
+      <c r="AA1" s="22"/>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A2" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
       <c r="G2" s="5"/>
-      <c r="H2" s="22" t="s">
+      <c r="H2" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
       <c r="N2" s="2"/>
-      <c r="O2" s="22" t="s">
+      <c r="O2" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="P2" s="22"/>
-      <c r="Q2" s="22"/>
-      <c r="R2" s="22"/>
-      <c r="S2" s="22"/>
-      <c r="T2" s="22"/>
+      <c r="P2" s="21"/>
+      <c r="Q2" s="21"/>
+      <c r="R2" s="21"/>
+      <c r="S2" s="21"/>
+      <c r="T2" s="21"/>
       <c r="U2" s="2"/>
-      <c r="V2" s="22" t="s">
+      <c r="V2" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="W2" s="22"/>
-      <c r="X2" s="22"/>
-      <c r="Y2" s="22"/>
-      <c r="Z2" s="22"/>
-      <c r="AA2" s="22"/>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="W2" s="21"/>
+      <c r="X2" s="21"/>
+      <c r="Y2" s="21"/>
+      <c r="Z2" s="21"/>
+      <c r="AA2" s="21"/>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -12537,7 +12537,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2004</v>
       </c>
@@ -12611,7 +12611,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>2005</v>
       </c>
@@ -12685,7 +12685,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>2006</v>
       </c>
@@ -12759,7 +12759,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>2007</v>
       </c>
@@ -12833,7 +12833,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>2008</v>
       </c>
@@ -12907,7 +12907,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>2009</v>
       </c>
@@ -12981,7 +12981,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>2010</v>
       </c>
@@ -13055,7 +13055,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>2011</v>
       </c>
@@ -13129,7 +13129,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>2012</v>
       </c>
@@ -13203,7 +13203,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>2013</v>
       </c>
@@ -13277,7 +13277,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>2014</v>
       </c>
@@ -13351,7 +13351,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>2015</v>
       </c>
@@ -13425,7 +13425,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A16" s="7">
         <v>2016</v>
       </c>
@@ -13490,30 +13490,30 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="O17" s="1"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="22" t="s">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A18" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="22"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
       <c r="G18" s="3"/>
-      <c r="O18" s="22" t="s">
+      <c r="O18" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="P18" s="22"/>
-      <c r="Q18" s="22"/>
-      <c r="R18" s="22"/>
-      <c r="S18" s="22"/>
-      <c r="T18" s="22"/>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="P18" s="21"/>
+      <c r="Q18" s="21"/>
+      <c r="R18" s="21"/>
+      <c r="S18" s="21"/>
+      <c r="T18" s="21"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A19" s="6" t="s">
         <v>1</v>
       </c>
@@ -13551,7 +13551,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>2004</v>
       </c>
@@ -13589,7 +13589,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>2005</v>
       </c>
@@ -13627,7 +13627,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>2006</v>
       </c>
@@ -13665,7 +13665,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>2007</v>
       </c>
@@ -13703,7 +13703,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>2008</v>
       </c>
@@ -13741,7 +13741,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>2009</v>
       </c>
@@ -13779,7 +13779,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>2010</v>
       </c>
@@ -13817,7 +13817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>2011</v>
       </c>
@@ -13855,7 +13855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>2012</v>
       </c>
@@ -13893,7 +13893,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>2013</v>
       </c>
@@ -13931,7 +13931,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>2014</v>
       </c>
@@ -13969,7 +13969,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>2015</v>
       </c>
@@ -14007,7 +14007,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A32" s="7">
         <v>2016</v>
       </c>
@@ -14046,43 +14046,43 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="23" t="s">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A36" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="B36" s="23"/>
-      <c r="C36" s="23"/>
-      <c r="D36" s="23"/>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
-      <c r="G36" s="23"/>
-      <c r="H36" s="23"/>
-      <c r="I36" s="23"/>
-      <c r="J36" s="23"/>
-      <c r="K36" s="23"/>
-      <c r="L36" s="23"/>
-      <c r="M36" s="23"/>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" s="22" t="s">
+      <c r="B36" s="22"/>
+      <c r="C36" s="22"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="22"/>
+      <c r="F36" s="22"/>
+      <c r="G36" s="22"/>
+      <c r="H36" s="22"/>
+      <c r="I36" s="22"/>
+      <c r="J36" s="22"/>
+      <c r="K36" s="22"/>
+      <c r="L36" s="22"/>
+      <c r="M36" s="22"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A37" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B37" s="22"/>
-      <c r="C37" s="22"/>
-      <c r="D37" s="22"/>
-      <c r="E37" s="22"/>
-      <c r="F37" s="22"/>
+      <c r="B37" s="21"/>
+      <c r="C37" s="21"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
       <c r="G37" s="5"/>
-      <c r="H37" s="22" t="s">
+      <c r="H37" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I37" s="22"/>
-      <c r="J37" s="22"/>
-      <c r="K37" s="22"/>
-      <c r="L37" s="22"/>
-      <c r="M37" s="22"/>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I37" s="21"/>
+      <c r="J37" s="21"/>
+      <c r="K37" s="21"/>
+      <c r="L37" s="21"/>
+      <c r="M37" s="21"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A38" s="6" t="s">
         <v>1</v>
       </c>
@@ -14120,7 +14120,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>2004</v>
       </c>
@@ -14158,7 +14158,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>2005</v>
       </c>
@@ -14196,7 +14196,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>2006</v>
       </c>
@@ -14234,7 +14234,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>2007</v>
       </c>
@@ -14272,7 +14272,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>2008</v>
       </c>
@@ -14310,7 +14310,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>2009</v>
       </c>
@@ -14348,7 +14348,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>2010</v>
       </c>
@@ -14386,7 +14386,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>2011</v>
       </c>
@@ -14424,7 +14424,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>2012</v>
       </c>
@@ -14462,7 +14462,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>2013</v>
       </c>
@@ -14500,7 +14500,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>2014</v>
       </c>
@@ -14538,7 +14538,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
         <v>2015</v>
       </c>
@@ -14576,7 +14576,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A51" s="7">
         <v>2016</v>
       </c>
@@ -14615,21 +14615,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A52" s="1"/>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A53" s="22" t="s">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A53" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B53" s="22"/>
-      <c r="C53" s="22"/>
-      <c r="D53" s="22"/>
-      <c r="E53" s="22"/>
-      <c r="F53" s="22"/>
+      <c r="B53" s="21"/>
+      <c r="C53" s="21"/>
+      <c r="D53" s="21"/>
+      <c r="E53" s="21"/>
+      <c r="F53" s="21"/>
       <c r="G53" s="3"/>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A54" s="6" t="s">
         <v>1</v>
       </c>
@@ -14649,7 +14649,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
         <v>2004</v>
       </c>
@@ -14669,7 +14669,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
         <v>2005</v>
       </c>
@@ -14689,7 +14689,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
         <v>2006</v>
       </c>
@@ -14709,7 +14709,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
         <v>2007</v>
       </c>
@@ -14729,7 +14729,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
         <v>2008</v>
       </c>
@@ -14749,7 +14749,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
         <v>2009</v>
       </c>
@@ -14769,7 +14769,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
         <v>2010</v>
       </c>
@@ -14789,7 +14789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
         <v>2011</v>
       </c>
@@ -14809,7 +14809,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
         <v>2012</v>
       </c>
@@ -14829,7 +14829,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
         <v>2013</v>
       </c>
@@ -14849,7 +14849,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <v>2014</v>
       </c>
@@ -14869,7 +14869,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
         <v>2015</v>
       </c>
@@ -14889,7 +14889,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A67" s="7">
         <v>2016</v>
       </c>

</xml_diff>